<commit_message>
Arregle importar beneficiarios y apoyos
</commit_message>
<xml_diff>
--- a/insezacweb/assets/files/subprogramas.xlsx
+++ b/insezacweb/assets/files/subprogramas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\INSEZAC\Archivos de proyecto\Catalogos pruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\INSEZAC\Archivos de proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="349">
   <si>
     <t>Subprograma</t>
   </si>
@@ -222,6 +222,855 @@
   </si>
   <si>
     <t>2 - Económicos</t>
+  </si>
+  <si>
+    <t>3J - Regulación, Conducción, Fomento Industrial y Promoción Industrial</t>
+  </si>
+  <si>
+    <t>5K - Edificios Administrativos</t>
+  </si>
+  <si>
+    <t>1 - Rehabilitación</t>
+  </si>
+  <si>
+    <t>2 - Ampliación</t>
+  </si>
+  <si>
+    <t>3 - Construcción</t>
+  </si>
+  <si>
+    <t>4 - Conservación</t>
+  </si>
+  <si>
+    <t>EV - Plantas Industriales</t>
+  </si>
+  <si>
+    <t>1 - Industria Agropecuaria</t>
+  </si>
+  <si>
+    <t>2 - Industria Textil</t>
+  </si>
+  <si>
+    <t>3 - Industria Alimenticia y Bebidas</t>
+  </si>
+  <si>
+    <t>4 - Industria Metal Mecánica</t>
+  </si>
+  <si>
+    <t>5 - Industria para la Construcción</t>
+  </si>
+  <si>
+    <t>FD - Producción y Transformación Agro-Industrial</t>
+  </si>
+  <si>
+    <t>1 - Rehabilitación - Ampliación</t>
+  </si>
+  <si>
+    <t>2 - Contrucción de Rastros</t>
+  </si>
+  <si>
+    <t>RG - Acciones Relevantes</t>
+  </si>
+  <si>
+    <t>1 - Proyectos Especiales.</t>
+  </si>
+  <si>
+    <t>S3 - Vivienda Progresiva</t>
+  </si>
+  <si>
+    <t>1 - Pie De Casa</t>
+  </si>
+  <si>
+    <t>2 - Lote de Material</t>
+  </si>
+  <si>
+    <t>3 - Reserva Territorial</t>
+  </si>
+  <si>
+    <t>S4 - Atención Preventiva y Curativa (Passpa)</t>
+  </si>
+  <si>
+    <t>1 - Atención Preventiva</t>
+  </si>
+  <si>
+    <t>2 - Atención Curativa</t>
+  </si>
+  <si>
+    <t>3 - Investigación para la Atención Preventiva y Curativa.</t>
+  </si>
+  <si>
+    <t>4 - Capacitación para la Atención Preventiva y Curativa.</t>
+  </si>
+  <si>
+    <t>S5 - Protección y Preservación Ecológica</t>
+  </si>
+  <si>
+    <t>01 OA - Tratamiento de Aguas Residuales Laguna de Oxidación</t>
+  </si>
+  <si>
+    <t>01 OB - Tratamiento de Aguas Residuales Laguna de Estabilización</t>
+  </si>
+  <si>
+    <t>02 OA - Manejo de Residuos Solidos Residuos Sólidos</t>
+  </si>
+  <si>
+    <t>02 OB - Manejo de Residuos Solidos Relleno Sanitario</t>
+  </si>
+  <si>
+    <t>3 - Protección del Medio Ambiente</t>
+  </si>
+  <si>
+    <t>4 - Reforestación</t>
+  </si>
+  <si>
+    <t>5 - Estudios y Proyectos</t>
+  </si>
+  <si>
+    <t>6 - Protección de la Flora y Fauna</t>
+  </si>
+  <si>
+    <t>7 - Remediación de Pasivos Ambientales</t>
+  </si>
+  <si>
+    <t>SA - Programa de Apoyo al Servicio Social</t>
+  </si>
+  <si>
+    <t>1 - Becas e Intercambio Educativo</t>
+  </si>
+  <si>
+    <t>SB - Estimulos a la Educación Basica</t>
+  </si>
+  <si>
+    <t>1 - Apoyo a la Educación Básica</t>
+  </si>
+  <si>
+    <t>SC - Agua Potable</t>
+  </si>
+  <si>
+    <t>4 - Conducción Agua Potable</t>
+  </si>
+  <si>
+    <t>5 - Dotación de Agua Potable</t>
+  </si>
+  <si>
+    <t>6 - Perforación de Pozo Profundo</t>
+  </si>
+  <si>
+    <t>7 - Equipamiento / Electrificación</t>
+  </si>
+  <si>
+    <t>SD - Alcantarillado</t>
+  </si>
+  <si>
+    <t>03 OA - Construcción Sistema</t>
+  </si>
+  <si>
+    <t>03 OB - Construcción Letrinización</t>
+  </si>
+  <si>
+    <t>SE - Urbanización</t>
+  </si>
+  <si>
+    <t>1 - Construcción de Calles</t>
+  </si>
+  <si>
+    <t>2 - Empedrado y Adoquinado de Calles</t>
+  </si>
+  <si>
+    <t>03 OA - Construcción de Guarniciones y Banquetas</t>
+  </si>
+  <si>
+    <t>03 OB - Construcción Muros de Contención</t>
+  </si>
+  <si>
+    <t>4 - Construcción Plazas Civicas y Jardines</t>
+  </si>
+  <si>
+    <t>05 OA - Alumbrado Público Poblado Rural</t>
+  </si>
+  <si>
+    <t>05 OB - Alumbrado Público Colonia Popular</t>
+  </si>
+  <si>
+    <t>06 OA - Construcción Pasos Peatonales</t>
+  </si>
+  <si>
+    <t>06 OB - Construcción Pasos Vehiculares</t>
+  </si>
+  <si>
+    <t>7 - Edificios Públicos</t>
+  </si>
+  <si>
+    <t>8 - Señalamientos</t>
+  </si>
+  <si>
+    <t>9 - Conservación, Rehabilitación y Mantenimiento</t>
+  </si>
+  <si>
+    <t>10 - Mejoramiento Urbano</t>
+  </si>
+  <si>
+    <t>SF - Pavimentación</t>
+  </si>
+  <si>
+    <t>1 - Concreto Hidráulico</t>
+  </si>
+  <si>
+    <t>2 - Concreto Asfaltico</t>
+  </si>
+  <si>
+    <t>SG - Electrificación</t>
+  </si>
+  <si>
+    <t>01 OA - Urbana (Colonias Pobres) Construcción</t>
+  </si>
+  <si>
+    <t>01 OB - Urbana (Colonias Pobres) Ampliación</t>
+  </si>
+  <si>
+    <t>01 OC - Urbana (Colonias Pobres) Obra Complementaria</t>
+  </si>
+  <si>
+    <t>02 OA - Rural Construcción</t>
+  </si>
+  <si>
+    <t>02 OB - Rural Ampliación</t>
+  </si>
+  <si>
+    <t>02 OC - Rural Obra Complementaria</t>
+  </si>
+  <si>
+    <t>03 OA - Pozos Agrí­colas - Lineas De Transmisión</t>
+  </si>
+  <si>
+    <t>04 OA - No Convencional (Planta de Luz)</t>
+  </si>
+  <si>
+    <t>SH - Vivienda Digna</t>
+  </si>
+  <si>
+    <t>01 OA - Rehabilitación Urbana</t>
+  </si>
+  <si>
+    <t>01 OB - Rehabilitación Rural</t>
+  </si>
+  <si>
+    <t>02 OA - Ampliación Urbana</t>
+  </si>
+  <si>
+    <t>02 OB - Ampliación Rural</t>
+  </si>
+  <si>
+    <t>03 OA - Construcción Urbana</t>
+  </si>
+  <si>
+    <t>03 OB - Construcción Rural</t>
+  </si>
+  <si>
+    <t>08 OA - Equipamiento Letrina</t>
+  </si>
+  <si>
+    <t>08 OB - Equipamiento Fogones</t>
+  </si>
+  <si>
+    <t>08 OC - Equipamiento Filtros de Agua</t>
+  </si>
+  <si>
+    <t>08 OD - Equipamiento Captadora de Agua</t>
+  </si>
+  <si>
+    <t>08 OE - Equipamiento Depósito de Agua</t>
+  </si>
+  <si>
+    <t>08 OF - Equipamiento Tinaco</t>
+  </si>
+  <si>
+    <t>08 OG - Equipamiento Cisterna</t>
+  </si>
+  <si>
+    <t>08 OH - Equipamiento Fosa Séptica</t>
+  </si>
+  <si>
+    <t>08 OI - Equipamento Biodigestor</t>
+  </si>
+  <si>
+    <t>08 OJ - Equipamento Estufa de Gas</t>
+  </si>
+  <si>
+    <t>08 OK - Equipamiento Calentador Solar</t>
+  </si>
+  <si>
+    <t>08 OL - Equipamiento Planta Solar</t>
+  </si>
+  <si>
+    <t>SI - Vialidades Urbanas</t>
+  </si>
+  <si>
+    <t>1 - Reconstrucción</t>
+  </si>
+  <si>
+    <t>2 - Modernización y Ampliación</t>
+  </si>
+  <si>
+    <t>4 - Conservación Y Mantenimiento</t>
+  </si>
+  <si>
+    <t>SJ - Infraestructura Educativa</t>
+  </si>
+  <si>
+    <t>4 - Equipamiento</t>
+  </si>
+  <si>
+    <t>SK - Escuela Digna</t>
+  </si>
+  <si>
+    <t>01 OA - Preescolar - Rehabilitación</t>
+  </si>
+  <si>
+    <t>01 OB - Preescolar - Equipamiento</t>
+  </si>
+  <si>
+    <t>02 OA - Primaria - Rehabilitación</t>
+  </si>
+  <si>
+    <t>02 OB - Primaria - Equipamiento</t>
+  </si>
+  <si>
+    <t>03 OA - Secundaria - Rehabilitación</t>
+  </si>
+  <si>
+    <t>03 OB - Secundaria - Equipamiento</t>
+  </si>
+  <si>
+    <t>04 OA - Otros Niveles - Rehabilitación</t>
+  </si>
+  <si>
+    <t>04 OB - Otros Niveles - Equipamiento</t>
+  </si>
+  <si>
+    <t>SL - Infraestructura Deportiva</t>
+  </si>
+  <si>
+    <t>5 - Obras Complementarias</t>
+  </si>
+  <si>
+    <t>SN - Infraestructura Hospitalaria</t>
+  </si>
+  <si>
+    <t>1 - Rehabilitación Mayor</t>
+  </si>
+  <si>
+    <t>SO - Centros de Salud</t>
+  </si>
+  <si>
+    <t>5 - Unidades Móviles</t>
+  </si>
+  <si>
+    <t>SP - Unidades Medicas Rurales</t>
+  </si>
+  <si>
+    <t>SQ - Centros de Bienestar Social</t>
+  </si>
+  <si>
+    <t>2 - Otros</t>
+  </si>
+  <si>
+    <t>SR - Ecología Productiva</t>
+  </si>
+  <si>
+    <t>1 - Proyectos Ecológicos Productivos</t>
+  </si>
+  <si>
+    <t>SS - Asistencia Social y Servicios Comunitarios</t>
+  </si>
+  <si>
+    <t>1 - Nutrición, Alimentación Y Salud</t>
+  </si>
+  <si>
+    <t>2 - Asistencia Social a la Niñez</t>
+  </si>
+  <si>
+    <t>3 - Asistencia Social a la Juventud</t>
+  </si>
+  <si>
+    <t>4 - Asistencia Social a la Senectud</t>
+  </si>
+  <si>
+    <t>5 - Procuración de Justicia al Indí­gena</t>
+  </si>
+  <si>
+    <t>6 - Desarrollo Comunitario</t>
+  </si>
+  <si>
+    <t>7 - Apoyo a la Educación de Adultos</t>
+  </si>
+  <si>
+    <t>8 - Asistencia Social a las Mujeres</t>
+  </si>
+  <si>
+    <t>9 - Educación, Capacitación y Formación</t>
+  </si>
+  <si>
+    <t>ST - Abasto y Comercialización</t>
+  </si>
+  <si>
+    <t>2 - Adaptación</t>
+  </si>
+  <si>
+    <t>4 - Recapitalización</t>
+  </si>
+  <si>
+    <t>TA - Fondos Sociales para la Producción</t>
+  </si>
+  <si>
+    <t>1 - Apoyos a la Producción</t>
+  </si>
+  <si>
+    <t>TB - Mujeres</t>
+  </si>
+  <si>
+    <t>1 - Proyectos Productivos</t>
+  </si>
+  <si>
+    <t>2 - Otros Proyectos</t>
+  </si>
+  <si>
+    <t>TC - Programas de Apoyo a Empresas Sociales</t>
+  </si>
+  <si>
+    <t>1 - Agrí­cola</t>
+  </si>
+  <si>
+    <t>2 - Agroindustrial</t>
+  </si>
+  <si>
+    <t>3 - Empresa Extractiva</t>
+  </si>
+  <si>
+    <t>4 - Microempresas</t>
+  </si>
+  <si>
+    <t>5 - Pecuarias, Forestales y Pesqueras</t>
+  </si>
+  <si>
+    <t>6 - Comercializadoras</t>
+  </si>
+  <si>
+    <t>TD - Fondos Sociales para el Desarrollo de los Pueblos Indigenas</t>
+  </si>
+  <si>
+    <t>1 - Agricola</t>
+  </si>
+  <si>
+    <t>2 - Pecuario</t>
+  </si>
+  <si>
+    <t>3 - Pesquero y Acuí­cola</t>
+  </si>
+  <si>
+    <t>4 - Silví­cola</t>
+  </si>
+  <si>
+    <t>5 - Agroindustrial</t>
+  </si>
+  <si>
+    <t>6 - Artesanal</t>
+  </si>
+  <si>
+    <t>7 - Otras Actividades</t>
+  </si>
+  <si>
+    <t>TE - Apoyo a la Producción Primaria</t>
+  </si>
+  <si>
+    <t>1 - Productores Agrí­colas</t>
+  </si>
+  <si>
+    <t>2 - Productores Pecuarios</t>
+  </si>
+  <si>
+    <t>3 - Productores Forestales</t>
+  </si>
+  <si>
+    <t>4 - Productores Pesqueros Y Acuí­colas</t>
+  </si>
+  <si>
+    <t>5 - Mineria Social</t>
+  </si>
+  <si>
+    <t>TF - Fomento a la Producción y Productividad</t>
+  </si>
+  <si>
+    <t>3 - Forestal</t>
+  </si>
+  <si>
+    <t>4 - Agroindustrial</t>
+  </si>
+  <si>
+    <t>5 - Artesanal</t>
+  </si>
+  <si>
+    <t>6 - Microempresa</t>
+  </si>
+  <si>
+    <t>7 - Industria Manufacturera Comunitaria</t>
+  </si>
+  <si>
+    <t>8 - Apoyo a la Elaboración de Materiales para la Contrucción</t>
+  </si>
+  <si>
+    <t>9 - Fomento a las Empresas Familiares o Comunitarias</t>
+  </si>
+  <si>
+    <t>10 - Formación de Capital Social</t>
+  </si>
+  <si>
+    <t>TG - Desarrollo Areas de Riego (Pequeña Irrigación)</t>
+  </si>
+  <si>
+    <t>2 - Construcción</t>
+  </si>
+  <si>
+    <t>3 - Nivelación de Tierrs</t>
+  </si>
+  <si>
+    <t>4 - Obras Complementarias</t>
+  </si>
+  <si>
+    <t>TH - Desarrollo de Areas de Temporal</t>
+  </si>
+  <si>
+    <t>1 - Desmonte</t>
+  </si>
+  <si>
+    <t>2 - Despiedre</t>
+  </si>
+  <si>
+    <t>3 - Nivelación de Tierra</t>
+  </si>
+  <si>
+    <t>4 - Subsuelo</t>
+  </si>
+  <si>
+    <t>5 - Conservación del Suelo y Agua</t>
+  </si>
+  <si>
+    <t>TI - Protección de Areas y Cauces Federales</t>
+  </si>
+  <si>
+    <t>1 - Areas Productivas</t>
+  </si>
+  <si>
+    <t>2 - Poblados</t>
+  </si>
+  <si>
+    <t>TJ - Infraestructura Pecuaria</t>
+  </si>
+  <si>
+    <t>TK - Regularización de Tenencia de la Tierra y Organización Agraria</t>
+  </si>
+  <si>
+    <t>2 - Asentamientos Humanos en Zona Rural</t>
+  </si>
+  <si>
+    <t>3 - Asentamientos Humanos en Zona Urbana</t>
+  </si>
+  <si>
+    <t>4 - Organización Agraria</t>
+  </si>
+  <si>
+    <t>TL - Regulación, Conducción y Fomento Industrial</t>
+  </si>
+  <si>
+    <t>1 - Promoción Industrial</t>
+  </si>
+  <si>
+    <t>2 - Industria Metal Mecánica</t>
+  </si>
+  <si>
+    <t>3 - Instrumentos y Mecanismos de Calidad</t>
+  </si>
+  <si>
+    <t>U5 - Tratamiento Aguas Residuales (Plantas de Tratamiento)</t>
+  </si>
+  <si>
+    <t>4 - Consolidación de la Infraestructura</t>
+  </si>
+  <si>
+    <t>U6 - Plantas Potabilizadoras</t>
+  </si>
+  <si>
+    <t>3 - Construción</t>
+  </si>
+  <si>
+    <t>U9 - Definición y Conducción de la Planeación del Desarrollo Regional</t>
+  </si>
+  <si>
+    <t>1 - Administración y Coordinación de la Planeación del Desarrollo Regional</t>
+  </si>
+  <si>
+    <t>2 - Control del Desarrollo Regional</t>
+  </si>
+  <si>
+    <t>3 - Evaluación del Desarrollo Regional</t>
+  </si>
+  <si>
+    <t>4 - Seguimiento del Desarrollo Regional</t>
+  </si>
+  <si>
+    <t>5 - Estudios y Proyectos para el Desarrollo Regional</t>
+  </si>
+  <si>
+    <t>6 - Evaluación y Seguimiento</t>
+  </si>
+  <si>
+    <t>7 - Administación</t>
+  </si>
+  <si>
+    <t>8 - Servicios</t>
+  </si>
+  <si>
+    <t>9 - Adquisiciones</t>
+  </si>
+  <si>
+    <t>10 - Promoción y Difusión</t>
+  </si>
+  <si>
+    <t>UB - Caminos Rurales</t>
+  </si>
+  <si>
+    <t>01 OA - Reconstrucción Caminos</t>
+  </si>
+  <si>
+    <t>01 OB - Reconstrucción Puentes</t>
+  </si>
+  <si>
+    <t>02 OA - Ampliación Caminos</t>
+  </si>
+  <si>
+    <t>02 OB - Ampliación Puentes</t>
+  </si>
+  <si>
+    <t>03 OA - Construcción Caminos</t>
+  </si>
+  <si>
+    <t>03 OB - Construcción Puentes</t>
+  </si>
+  <si>
+    <t>04 OA - Conservación Caminos</t>
+  </si>
+  <si>
+    <t>04 OB - Conservación Puentes</t>
+  </si>
+  <si>
+    <t>05 OA - Obras Complementarias Caminos</t>
+  </si>
+  <si>
+    <t>05 OB - Obras Complementarias Puentes</t>
+  </si>
+  <si>
+    <t>UC - Carreteras Alimentadoras</t>
+  </si>
+  <si>
+    <t>01 OA - Reconstrucción Carreteras</t>
+  </si>
+  <si>
+    <t>02 OA - Modernización y Ampliación Carreteras</t>
+  </si>
+  <si>
+    <t>02 OB - Modernización y Ampliación Puentes</t>
+  </si>
+  <si>
+    <t>03 OA - Construcción Carreteras</t>
+  </si>
+  <si>
+    <t>04 OA - Conservación Carreteras</t>
+  </si>
+  <si>
+    <t>5 - Estudios</t>
+  </si>
+  <si>
+    <t>6 - Obras Complementarias</t>
+  </si>
+  <si>
+    <t>UD - Infraestructura Aeroportuaria</t>
+  </si>
+  <si>
+    <t>2 - Modernización</t>
+  </si>
+  <si>
+    <t>UE - Sitios Históricos y Culturales</t>
+  </si>
+  <si>
+    <t>2 - Restauración - Conservación</t>
+  </si>
+  <si>
+    <t>3 - Administración</t>
+  </si>
+  <si>
+    <t>UF - Fomento al Turismo</t>
+  </si>
+  <si>
+    <t>1 - Rehabilitación de Infraestructura</t>
+  </si>
+  <si>
+    <t>2 - Ampliación de Infraestructura</t>
+  </si>
+  <si>
+    <t>3 - Construcción de Infraestructura</t>
+  </si>
+  <si>
+    <t>4 - Turismo Social</t>
+  </si>
+  <si>
+    <t>UG - Telefonía Rural</t>
+  </si>
+  <si>
+    <t>UH - Infraestructura Penitenciaria</t>
+  </si>
+  <si>
+    <t>5 - Dignificación</t>
+  </si>
+  <si>
+    <t>UI - Seguridad Pública</t>
+  </si>
+  <si>
+    <t>5 - Capacitación - Certificación</t>
+  </si>
+  <si>
+    <t>6 - Otros Conceptos</t>
+  </si>
+  <si>
+    <t>UJ - Despresurización Penitenciaria</t>
+  </si>
+  <si>
+    <t>1 - Despresurización</t>
+  </si>
+  <si>
+    <t>UK - Becas de Capacitación para Trabajadores</t>
+  </si>
+  <si>
+    <t>1 - Becas</t>
+  </si>
+  <si>
+    <t>UL - Servicio Estatal de Empleo</t>
+  </si>
+  <si>
+    <t>1 - Capacitación</t>
+  </si>
+  <si>
+    <t>2 - Becas</t>
+  </si>
+  <si>
+    <t>3 - Apoyos</t>
+  </si>
+  <si>
+    <t>US - Unidad de Servicios Integrales</t>
+  </si>
+  <si>
+    <t>01 OA - Rehabilitación Cocina- Comedor</t>
+  </si>
+  <si>
+    <t>01 OB - Rehabilitación Módulo Sanitario</t>
+  </si>
+  <si>
+    <t>01 OC - Rehabilitación Módulo de Salud</t>
+  </si>
+  <si>
+    <t>01 OD - Rehabilitación Dormitorios</t>
+  </si>
+  <si>
+    <t>02 OA - Ampliación Cocina- Comedor</t>
+  </si>
+  <si>
+    <t>02 OB - Ampliación Módulo Sanitario</t>
+  </si>
+  <si>
+    <t>02 OC - Ampliación Módulo de Salud</t>
+  </si>
+  <si>
+    <t>02 OD - Ampliación Dormitorios</t>
+  </si>
+  <si>
+    <t>03 OA - Construcción Cocina - Comedor</t>
+  </si>
+  <si>
+    <t>03 OB - Construcción Módulo Sanitario</t>
+  </si>
+  <si>
+    <t>03 OC - Construcción Módulo de Salud</t>
+  </si>
+  <si>
+    <t>03 OD - Construcción Dormitorios</t>
+  </si>
+  <si>
+    <t>03 OE - Construcción Obra Complementaria</t>
+  </si>
+  <si>
+    <t>UT - Zonas de Riego</t>
+  </si>
+  <si>
+    <t>01 OA - Rehabilitacion de Bordo.</t>
+  </si>
+  <si>
+    <t>01 OB - Rehabilitacion de Canal.</t>
+  </si>
+  <si>
+    <t>02 OA - Ampliación de Bordo</t>
+  </si>
+  <si>
+    <t>02 OB - Ampliación de Canal</t>
+  </si>
+  <si>
+    <t>03 OA - Construccion de Bordo</t>
+  </si>
+  <si>
+    <t>03 OB - Construccion de Canal.</t>
+  </si>
+  <si>
+    <t>ZE - Acciones y Apoyos Educativos</t>
+  </si>
+  <si>
+    <t>1 - Educación Inicial</t>
+  </si>
+  <si>
+    <t>03 OA - Educación Preescolar Federalizado</t>
+  </si>
+  <si>
+    <t>03 OB - Educación Preescolar Estatal</t>
+  </si>
+  <si>
+    <t>4 - Educación Primaria</t>
+  </si>
+  <si>
+    <t>7 - Educación Básica</t>
+  </si>
+  <si>
+    <t>8 - Educación Básica para Adultos</t>
+  </si>
+  <si>
+    <t>14 OA - Sistema de Becas Federalizado</t>
+  </si>
+  <si>
+    <t>14 OB - Sistema de Becas Estatal</t>
+  </si>
+  <si>
+    <t>16 OA - Administración de Servicios Educativos Federalizados</t>
+  </si>
+  <si>
+    <t>16 OB - Administración de Servicios Educativos Estatales</t>
+  </si>
+  <si>
+    <t>19 - Educación Media Superior</t>
+  </si>
+  <si>
+    <t>20 OA - Educación Superior Federalizada</t>
+  </si>
+  <si>
+    <t>20 OB - Educación Superior Estatal</t>
+  </si>
+  <si>
+    <t>21 - Equidad de Género</t>
   </si>
 </sst>
 </file>
@@ -256,7 +1105,7 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -273,6 +1122,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -331,16 +1186,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -622,10 +1480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D365"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,16 +1503,16 @@
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1706,6 +2564,4038 @@
       </c>
       <c r="D77" s="1" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C78" s="1">
+        <v>10</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C79" s="1">
+        <v>10</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C80" s="1">
+        <v>11</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C81" s="1">
+        <v>11</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C82" s="1">
+        <v>11</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C83" s="1">
+        <v>11</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C84" s="1">
+        <v>12</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C85" s="1">
+        <v>12</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C86" s="1">
+        <v>12</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C87" s="1">
+        <v>12</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C88" s="1">
+        <v>12</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C89" s="1">
+        <v>13</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C90" s="1">
+        <v>13</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C91" s="1">
+        <v>14</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C92" s="1">
+        <v>15</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C93" s="1">
+        <v>15</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C94" s="1">
+        <v>15</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C95" s="1">
+        <v>16</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C96" s="1">
+        <v>16</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C97" s="1">
+        <v>16</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C98" s="1">
+        <v>16</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C99" s="1">
+        <v>17</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C100" s="1">
+        <v>17</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C101" s="1">
+        <v>17</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>100</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C102" s="1">
+        <v>17</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>101</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C103" s="1">
+        <v>17</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>102</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C104" s="1">
+        <v>17</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>103</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C105" s="1">
+        <v>17</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>104</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C106" s="1">
+        <v>17</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>105</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C107" s="1">
+        <v>17</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>106</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C108" s="1">
+        <v>18</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>107</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C109" s="1">
+        <v>19</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>108</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C110" s="1">
+        <v>20</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>109</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C111" s="1">
+        <v>20</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>110</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C112" s="1">
+        <v>20</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>111</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C113" s="1">
+        <v>20</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>112</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C114" s="1">
+        <v>20</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>113</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C115" s="1">
+        <v>20</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>114</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C116" s="1">
+        <v>20</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>115</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C117" s="1">
+        <v>21</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>116</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C118" s="1">
+        <v>21</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>117</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C119" s="1">
+        <v>21</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>118</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C120" s="1">
+        <v>21</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>119</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C121" s="1">
+        <v>22</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>120</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C122" s="1">
+        <v>22</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>121</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C123" s="1">
+        <v>22</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>122</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C124" s="1">
+        <v>22</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>123</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C125" s="1">
+        <v>22</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>124</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C126" s="1">
+        <v>22</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>125</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C127" s="1">
+        <v>22</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>126</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C128" s="1">
+        <v>22</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>127</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C129" s="1">
+        <v>22</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>128</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C130" s="1">
+        <v>22</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>129</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C131" s="1">
+        <v>22</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>130</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C132" s="1">
+        <v>22</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>131</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C133" s="1">
+        <v>22</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>132</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C134" s="1">
+        <v>23</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>133</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C135" s="1">
+        <v>23</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>134</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C136" s="1">
+        <v>24</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>135</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C137" s="1">
+        <v>24</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>136</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C138" s="1">
+        <v>24</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>137</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C139" s="1">
+        <v>24</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>138</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C140" s="1">
+        <v>24</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>139</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C141" s="1">
+        <v>24</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>140</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C142" s="1">
+        <v>24</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>141</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C143" s="1">
+        <v>24</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>142</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C144" s="1">
+        <v>25</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>143</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C145" s="1">
+        <v>25</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>144</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C146" s="1">
+        <v>25</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>145</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C147" s="1">
+        <v>25</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>146</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C148" s="1">
+        <v>25</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>147</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C149" s="1">
+        <v>25</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <v>352</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C150" s="1">
+        <v>25</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>353</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C151" s="1">
+        <v>25</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>354</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C152" s="1">
+        <v>25</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <v>355</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C153" s="1">
+        <v>25</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>356</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C154" s="1">
+        <v>25</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>357</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C155" s="1">
+        <v>25</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <v>358</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C156" s="1">
+        <v>25</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>359</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C157" s="1">
+        <v>25</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>360</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C158" s="1">
+        <v>25</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>361</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C159" s="1">
+        <v>25</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>362</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C160" s="1">
+        <v>25</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>363</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C161" s="1">
+        <v>25</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <v>148</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C162" s="1">
+        <v>26</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <v>149</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C163" s="1">
+        <v>26</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>150</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C164" s="1">
+        <v>26</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <v>151</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C165" s="1">
+        <v>26</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <v>152</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C166" s="1">
+        <v>27</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>153</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C167" s="1">
+        <v>27</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="1">
+        <v>154</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C168" s="1">
+        <v>27</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="1">
+        <v>155</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C169" s="1">
+        <v>27</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="1">
+        <v>156</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C170" s="1">
+        <v>28</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="1">
+        <v>157</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C171" s="1">
+        <v>28</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <v>158</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C172" s="1">
+        <v>28</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <v>159</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C173" s="1">
+        <v>28</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="1">
+        <v>160</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C174" s="1">
+        <v>28</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="1">
+        <v>161</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C175" s="1">
+        <v>28</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="1">
+        <v>162</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C176" s="1">
+        <v>28</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <v>163</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C177" s="1">
+        <v>28</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="1">
+        <v>164</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C178" s="1">
+        <v>29</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="1">
+        <v>165</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C179" s="1">
+        <v>29</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
+        <v>166</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C180" s="1">
+        <v>29</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="1">
+        <v>167</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C181" s="1">
+        <v>29</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="1">
+        <v>168</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C182" s="1">
+        <v>29</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="1">
+        <v>169</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C183" s="1">
+        <v>30</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>170</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C184" s="1">
+        <v>30</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>171</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C185" s="1">
+        <v>30</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>172</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C186" s="1">
+        <v>30</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <v>173</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C187" s="1">
+        <v>31</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <v>174</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C188" s="1">
+        <v>31</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>175</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C189" s="1">
+        <v>31</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>176</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C190" s="1">
+        <v>31</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>177</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C191" s="1">
+        <v>31</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>178</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C192" s="1">
+        <v>32</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>179</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C193" s="1">
+        <v>32</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>180</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C194" s="1">
+        <v>33</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>181</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C195" s="1">
+        <v>33</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <v>182</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C196" s="1">
+        <v>34</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>183</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C197" s="1">
+        <v>35</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>184</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C198" s="1">
+        <v>35</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <v>185</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C199" s="1">
+        <v>35</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>186</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C200" s="1">
+        <v>35</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="1">
+        <v>187</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C201" s="1">
+        <v>35</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
+        <v>188</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C202" s="1">
+        <v>35</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="1">
+        <v>189</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C203" s="1">
+        <v>35</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
+        <v>190</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C204" s="1">
+        <v>35</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="1">
+        <v>191</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C205" s="1">
+        <v>35</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="1">
+        <v>192</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C206" s="1">
+        <v>36</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
+        <v>193</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C207" s="1">
+        <v>36</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>194</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C208" s="1">
+        <v>36</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" s="1">
+        <v>195</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C209" s="1">
+        <v>36</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="1">
+        <v>196</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C210" s="1">
+        <v>37</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="1">
+        <v>197</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C211" s="1">
+        <v>38</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="1">
+        <v>198</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C212" s="1">
+        <v>38</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="1">
+        <v>199</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C213" s="1">
+        <v>39</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="1">
+        <v>200</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C214" s="1">
+        <v>39</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" s="1">
+        <v>201</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C215" s="1">
+        <v>39</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" s="1">
+        <v>202</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C216" s="1">
+        <v>39</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="1">
+        <v>203</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C217" s="1">
+        <v>39</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" s="1">
+        <v>204</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C218" s="1">
+        <v>39</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="1">
+        <v>205</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C219" s="1">
+        <v>40</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" s="1">
+        <v>206</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C220" s="1">
+        <v>40</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" s="1">
+        <v>207</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C221" s="1">
+        <v>40</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" s="1">
+        <v>208</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C222" s="1">
+        <v>40</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" s="1">
+        <v>209</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C223" s="1">
+        <v>40</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" s="1">
+        <v>210</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C224" s="1">
+        <v>40</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" s="1">
+        <v>211</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C225" s="1">
+        <v>40</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" s="1">
+        <v>212</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C226" s="1">
+        <v>41</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" s="1">
+        <v>213</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C227" s="1">
+        <v>41</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="1">
+        <v>214</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C228" s="1">
+        <v>41</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" s="1">
+        <v>215</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C229" s="1">
+        <v>41</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" s="1">
+        <v>216</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C230" s="1">
+        <v>41</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" s="1">
+        <v>217</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C231" s="1">
+        <v>42</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" s="1">
+        <v>218</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C232" s="1">
+        <v>42</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" s="1">
+        <v>219</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C233" s="1">
+        <v>42</v>
+      </c>
+      <c r="D233" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" s="1">
+        <v>220</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C234" s="1">
+        <v>42</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" s="1">
+        <v>221</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C235" s="1">
+        <v>42</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" s="1">
+        <v>222</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C236" s="1">
+        <v>42</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" s="1">
+        <v>223</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C237" s="1">
+        <v>42</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" s="1">
+        <v>224</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C238" s="1">
+        <v>42</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" s="1">
+        <v>225</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C239" s="1">
+        <v>42</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" s="1">
+        <v>226</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C240" s="1">
+        <v>42</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" s="1">
+        <v>227</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C241" s="1">
+        <v>43</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="1">
+        <v>228</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C242" s="1">
+        <v>43</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" s="1">
+        <v>229</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C243" s="1">
+        <v>43</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" s="1">
+        <v>230</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C244" s="1">
+        <v>43</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" s="1">
+        <v>231</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C245" s="1">
+        <v>44</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" s="1">
+        <v>232</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C246" s="1">
+        <v>44</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" s="1">
+        <v>233</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C247" s="1">
+        <v>44</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" s="1">
+        <v>234</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C248" s="1">
+        <v>44</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" s="1">
+        <v>235</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C249" s="1">
+        <v>44</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" s="1">
+        <v>236</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C250" s="1">
+        <v>45</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" s="1">
+        <v>237</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C251" s="1">
+        <v>45</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" s="1">
+        <v>238</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C252" s="1">
+        <v>46</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" s="1">
+        <v>239</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C253" s="1">
+        <v>46</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" s="1">
+        <v>240</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C254" s="1">
+        <v>46</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" s="1">
+        <v>241</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C255" s="1">
+        <v>47</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" s="1">
+        <v>242</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C256" s="1">
+        <v>47</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" s="1">
+        <v>243</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C257" s="1">
+        <v>47</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" s="1">
+        <v>244</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C258" s="1">
+        <v>47</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" s="1">
+        <v>245</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C259" s="1">
+        <v>48</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" s="1">
+        <v>246</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C260" s="1">
+        <v>48</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" s="1">
+        <v>247</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C261" s="1">
+        <v>48</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" s="1">
+        <v>248</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C262" s="1">
+        <v>49</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" s="1">
+        <v>249</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C263" s="1">
+        <v>49</v>
+      </c>
+      <c r="D263" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" s="1">
+        <v>250</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C264" s="1">
+        <v>49</v>
+      </c>
+      <c r="D264" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" s="1">
+        <v>251</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C265" s="1">
+        <v>49</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" s="1">
+        <v>252</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C266" s="1">
+        <v>50</v>
+      </c>
+      <c r="D266" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" s="1">
+        <v>253</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C267" s="1">
+        <v>50</v>
+      </c>
+      <c r="D267" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" s="1">
+        <v>254</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C268" s="1">
+        <v>50</v>
+      </c>
+      <c r="D268" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" s="1">
+        <v>255</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C269" s="1">
+        <v>50</v>
+      </c>
+      <c r="D269" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" s="1">
+        <v>256</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C270" s="1">
+        <v>51</v>
+      </c>
+      <c r="D270" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" s="1">
+        <v>257</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C271" s="1">
+        <v>51</v>
+      </c>
+      <c r="D271" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" s="1">
+        <v>258</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C272" s="1">
+        <v>51</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" s="1">
+        <v>259</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C273" s="1">
+        <v>51</v>
+      </c>
+      <c r="D273" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" s="1">
+        <v>260</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C274" s="1">
+        <v>51</v>
+      </c>
+      <c r="D274" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" s="1">
+        <v>261</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C275" s="1">
+        <v>51</v>
+      </c>
+      <c r="D275" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" s="1">
+        <v>262</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C276" s="1">
+        <v>51</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" s="1">
+        <v>263</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C277" s="1">
+        <v>51</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" s="1">
+        <v>264</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C278" s="1">
+        <v>51</v>
+      </c>
+      <c r="D278" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" s="1">
+        <v>265</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C279" s="1">
+        <v>51</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" s="1">
+        <v>266</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C280" s="1">
+        <v>52</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A281" s="1">
+        <v>267</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C281" s="1">
+        <v>52</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282" s="1">
+        <v>268</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C282" s="1">
+        <v>52</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" s="1">
+        <v>269</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C283" s="1">
+        <v>52</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" s="1">
+        <v>270</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C284" s="1">
+        <v>52</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A285" s="1">
+        <v>271</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C285" s="1">
+        <v>52</v>
+      </c>
+      <c r="D285" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A286" s="1">
+        <v>272</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C286" s="1">
+        <v>52</v>
+      </c>
+      <c r="D286" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287" s="1">
+        <v>273</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C287" s="1">
+        <v>52</v>
+      </c>
+      <c r="D287" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288" s="1">
+        <v>274</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C288" s="1">
+        <v>52</v>
+      </c>
+      <c r="D288" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289" s="1">
+        <v>275</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C289" s="1">
+        <v>52</v>
+      </c>
+      <c r="D289" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" s="1">
+        <v>276</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C290" s="1">
+        <v>53</v>
+      </c>
+      <c r="D290" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" s="1">
+        <v>277</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C291" s="1">
+        <v>53</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292" s="1">
+        <v>278</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C292" s="1">
+        <v>53</v>
+      </c>
+      <c r="D292" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293" s="1">
+        <v>279</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C293" s="1">
+        <v>53</v>
+      </c>
+      <c r="D293" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A294" s="1">
+        <v>280</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C294" s="1">
+        <v>53</v>
+      </c>
+      <c r="D294" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A295" s="1">
+        <v>281</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C295" s="1">
+        <v>53</v>
+      </c>
+      <c r="D295" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296" s="1">
+        <v>282</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C296" s="1">
+        <v>53</v>
+      </c>
+      <c r="D296" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A297" s="1">
+        <v>283</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C297" s="1">
+        <v>53</v>
+      </c>
+      <c r="D297" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298" s="1">
+        <v>284</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C298" s="1">
+        <v>53</v>
+      </c>
+      <c r="D298" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299" s="1">
+        <v>285</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C299" s="1">
+        <v>53</v>
+      </c>
+      <c r="D299" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A300" s="1">
+        <v>286</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C300" s="1">
+        <v>54</v>
+      </c>
+      <c r="D300" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A301" s="1">
+        <v>287</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C301" s="1">
+        <v>54</v>
+      </c>
+      <c r="D301" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A302" s="1">
+        <v>288</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C302" s="1">
+        <v>55</v>
+      </c>
+      <c r="D302" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A303" s="1">
+        <v>289</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C303" s="1">
+        <v>55</v>
+      </c>
+      <c r="D303" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A304" s="1">
+        <v>290</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C304" s="1">
+        <v>55</v>
+      </c>
+      <c r="D304" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A305" s="1">
+        <v>291</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C305" s="1">
+        <v>56</v>
+      </c>
+      <c r="D305" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A306" s="1">
+        <v>292</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C306" s="1">
+        <v>56</v>
+      </c>
+      <c r="D306" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A307" s="1">
+        <v>293</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C307" s="1">
+        <v>56</v>
+      </c>
+      <c r="D307" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A308" s="1">
+        <v>294</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C308" s="1">
+        <v>56</v>
+      </c>
+      <c r="D308" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A309" s="1">
+        <v>295</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C309" s="1">
+        <v>57</v>
+      </c>
+      <c r="D309" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A310" s="1">
+        <v>296</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C310" s="1">
+        <v>57</v>
+      </c>
+      <c r="D310" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A311" s="1">
+        <v>297</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C311" s="1">
+        <v>57</v>
+      </c>
+      <c r="D311" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A312" s="1">
+        <v>298</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C312" s="1">
+        <v>58</v>
+      </c>
+      <c r="D312" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A313" s="1">
+        <v>299</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C313" s="1">
+        <v>58</v>
+      </c>
+      <c r="D313" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A314" s="1">
+        <v>300</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C314" s="1">
+        <v>58</v>
+      </c>
+      <c r="D314" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A315" s="1">
+        <v>301</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C315" s="1">
+        <v>58</v>
+      </c>
+      <c r="D315" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A316" s="1">
+        <v>302</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C316" s="1">
+        <v>58</v>
+      </c>
+      <c r="D316" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A317" s="1">
+        <v>303</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C317" s="1">
+        <v>59</v>
+      </c>
+      <c r="D317" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A318" s="1">
+        <v>304</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C318" s="1">
+        <v>59</v>
+      </c>
+      <c r="D318" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A319" s="1">
+        <v>305</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C319" s="1">
+        <v>59</v>
+      </c>
+      <c r="D319" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A320" s="1">
+        <v>306</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C320" s="1">
+        <v>59</v>
+      </c>
+      <c r="D320" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A321" s="1">
+        <v>307</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C321" s="1">
+        <v>59</v>
+      </c>
+      <c r="D321" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A322" s="1">
+        <v>308</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C322" s="1">
+        <v>59</v>
+      </c>
+      <c r="D322" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A323" s="1">
+        <v>309</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C323" s="1">
+        <v>60</v>
+      </c>
+      <c r="D323" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A324" s="1">
+        <v>310</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C324" s="1">
+        <v>61</v>
+      </c>
+      <c r="D324" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A325" s="2">
+        <v>311</v>
+      </c>
+      <c r="B325" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C325" s="2">
+        <v>62</v>
+      </c>
+      <c r="D325" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A326" s="2">
+        <v>312</v>
+      </c>
+      <c r="B326" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C326" s="2">
+        <v>62</v>
+      </c>
+      <c r="D326" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A327" s="2">
+        <v>313</v>
+      </c>
+      <c r="B327" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C327" s="2">
+        <v>62</v>
+      </c>
+      <c r="D327" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A328" s="1">
+        <v>314</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C328" s="1">
+        <v>63</v>
+      </c>
+      <c r="D328" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A329" s="1">
+        <v>315</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C329" s="1">
+        <v>63</v>
+      </c>
+      <c r="D329" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A330" s="1">
+        <v>316</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C330" s="1">
+        <v>63</v>
+      </c>
+      <c r="D330" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A331" s="1">
+        <v>317</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C331" s="1">
+        <v>63</v>
+      </c>
+      <c r="D331" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A332" s="1">
+        <v>318</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C332" s="1">
+        <v>63</v>
+      </c>
+      <c r="D332" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A333" s="1">
+        <v>319</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C333" s="1">
+        <v>63</v>
+      </c>
+      <c r="D333" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A334" s="1">
+        <v>320</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C334" s="1">
+        <v>63</v>
+      </c>
+      <c r="D334" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A335" s="1">
+        <v>321</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C335" s="1">
+        <v>63</v>
+      </c>
+      <c r="D335" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A336" s="1">
+        <v>322</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C336" s="1">
+        <v>63</v>
+      </c>
+      <c r="D336" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A337" s="1">
+        <v>323</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C337" s="1">
+        <v>63</v>
+      </c>
+      <c r="D337" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A338" s="1">
+        <v>324</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C338" s="1">
+        <v>63</v>
+      </c>
+      <c r="D338" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A339" s="1">
+        <v>325</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C339" s="1">
+        <v>63</v>
+      </c>
+      <c r="D339" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A340" s="1">
+        <v>326</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C340" s="1">
+        <v>63</v>
+      </c>
+      <c r="D340" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A341" s="1">
+        <v>327</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C341" s="1">
+        <v>63</v>
+      </c>
+      <c r="D341" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A342" s="1">
+        <v>328</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C342" s="1">
+        <v>63</v>
+      </c>
+      <c r="D342" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A343" s="1">
+        <v>329</v>
+      </c>
+      <c r="B343" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C343" s="1">
+        <v>63</v>
+      </c>
+      <c r="D343" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A344" s="1">
+        <v>330</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C344" s="1">
+        <v>63</v>
+      </c>
+      <c r="D344" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A345" s="1">
+        <v>331</v>
+      </c>
+      <c r="B345" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C345" s="1">
+        <v>63</v>
+      </c>
+      <c r="D345" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A346" s="1">
+        <v>332</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C346" s="1">
+        <v>64</v>
+      </c>
+      <c r="D346" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A347" s="1">
+        <v>333</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C347" s="1">
+        <v>64</v>
+      </c>
+      <c r="D347" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A348" s="1">
+        <v>334</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C348" s="1">
+        <v>64</v>
+      </c>
+      <c r="D348" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A349" s="1">
+        <v>335</v>
+      </c>
+      <c r="B349" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C349" s="1">
+        <v>64</v>
+      </c>
+      <c r="D349" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A350" s="1">
+        <v>336</v>
+      </c>
+      <c r="B350" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C350" s="1">
+        <v>64</v>
+      </c>
+      <c r="D350" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A351" s="1">
+        <v>337</v>
+      </c>
+      <c r="B351" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C351" s="1">
+        <v>64</v>
+      </c>
+      <c r="D351" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A352" s="1">
+        <v>338</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C352" s="1">
+        <v>65</v>
+      </c>
+      <c r="D352" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A353" s="1">
+        <v>339</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C353" s="1">
+        <v>65</v>
+      </c>
+      <c r="D353" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A354" s="1">
+        <v>340</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C354" s="1">
+        <v>65</v>
+      </c>
+      <c r="D354" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A355" s="1">
+        <v>341</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C355" s="1">
+        <v>65</v>
+      </c>
+      <c r="D355" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A356" s="1">
+        <v>342</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C356" s="1">
+        <v>65</v>
+      </c>
+      <c r="D356" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A357" s="1">
+        <v>343</v>
+      </c>
+      <c r="B357" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C357" s="1">
+        <v>65</v>
+      </c>
+      <c r="D357" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A358" s="1">
+        <v>344</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C358" s="1">
+        <v>65</v>
+      </c>
+      <c r="D358" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A359" s="1">
+        <v>345</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C359" s="1">
+        <v>65</v>
+      </c>
+      <c r="D359" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A360" s="1">
+        <v>346</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C360" s="1">
+        <v>65</v>
+      </c>
+      <c r="D360" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A361" s="1">
+        <v>347</v>
+      </c>
+      <c r="B361" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C361" s="1">
+        <v>65</v>
+      </c>
+      <c r="D361" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A362" s="1">
+        <v>348</v>
+      </c>
+      <c r="B362" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C362" s="1">
+        <v>65</v>
+      </c>
+      <c r="D362" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A363" s="1">
+        <v>349</v>
+      </c>
+      <c r="B363" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C363" s="1">
+        <v>65</v>
+      </c>
+      <c r="D363" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A364" s="1">
+        <v>350</v>
+      </c>
+      <c r="B364" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C364" s="1">
+        <v>65</v>
+      </c>
+      <c r="D364" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A365" s="1">
+        <v>351</v>
+      </c>
+      <c r="B365" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C365" s="1">
+        <v>65</v>
+      </c>
+      <c r="D365" s="1" t="s">
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>